<commit_message>
Data: - Actualización de las variables mensuales. - Eliminación de las gráficas exploratorias preliminares.
</commit_message>
<xml_diff>
--- a/data/variables/IDEAM_categorias_estacion_parametros_etiquetas.xlsx
+++ b/data/variables/IDEAM_categorias_estacion_parametros_etiquetas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Google Drive\DS4All_Team28\estaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Source\Repos\DS4All_2020_Team28_Project\data\variables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4438E1B4-7532-45D9-BEDD-DE3227EDBFCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B00746-3C07-4FC9-8C94-EABF746BCDEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6F3B24C6-7B74-482C-914A-5A1F96AD68FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="62">
   <si>
     <t>Limnimétrica</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>climatica_ordinaria.csv</t>
+  </si>
+  <si>
+    <t>media + 3dev</t>
+  </si>
+  <si>
+    <t>Min Neg</t>
+  </si>
+  <si>
+    <t>Max Neg</t>
+  </si>
+  <si>
+    <t>media - 3dev, Mayor que cero</t>
   </si>
 </sst>
 </file>
@@ -560,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0723CD-55F4-4AC0-8087-65ED1D234C64}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,15 +589,15 @@
     <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -613,8 +625,14 @@
       <c r="I1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -643,7 +661,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -669,7 +687,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -695,7 +713,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -721,7 +739,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -750,7 +768,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -776,7 +794,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -801,8 +819,14 @@
       <c r="I8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -828,7 +852,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -857,7 +881,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -886,7 +910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -912,7 +936,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -937,8 +961,14 @@
       <c r="I13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -967,7 +997,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -993,7 +1023,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>

</xml_diff>